<commit_message>
adicionando alterações finais da sprint 2 entregue 19.09
</commit_message>
<xml_diff>
--- a/Projeto Integrador - Sprints.xlsx
+++ b/Projeto Integrador - Sprints.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Desktop\DIGITAL HOUSE\Curso Full Stack\Projeto Integrador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Desktop\DIGITAL HOUSE\Curso Full Stack\Projeto-DH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17421CBB-718D-4EC6-85C1-02833D7BFC67}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE82EDF8-F040-466E-940B-5EC37428F6BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>SPRINT 1</t>
   </si>
@@ -81,20 +81,68 @@
     <t>Página 5 - LoginCadastros</t>
   </si>
   <si>
-    <t>Seleção de imagens para todas as páginas</t>
-  </si>
-  <si>
-    <t>Definição dos textos para todas as páginas</t>
-  </si>
-  <si>
-    <t>LOGO - definição do nome e elaboração do Logo</t>
+    <t>Entregue! (com algumas coisas faltantes)</t>
+  </si>
+  <si>
+    <t>Laura - OK</t>
+  </si>
+  <si>
+    <t>Stela - OK</t>
+  </si>
+  <si>
+    <t>Higor - OK</t>
+  </si>
+  <si>
+    <t>Sabrine - OK</t>
+  </si>
+  <si>
+    <t>Stela</t>
+  </si>
+  <si>
+    <t>Sabrine</t>
+  </si>
+  <si>
+    <t>Ajustar páginas com modelo da YELLOW</t>
+  </si>
+  <si>
+    <t>Melhorar CSS (cores, fontes, etc..)</t>
+  </si>
+  <si>
+    <t>Login - virar modal (php) - idem modelo dado em aula</t>
+  </si>
+  <si>
+    <t>Criar página de alteração do cadastro - após login</t>
+  </si>
+  <si>
+    <t>SPRINT 3</t>
+  </si>
+  <si>
+    <t>Finalização do Front-end + Back (php)</t>
+  </si>
+  <si>
+    <t>TEXTOS E TÍTULOS: Definição dos textos para todas as páginas</t>
+  </si>
+  <si>
+    <t>IMAGENS: Seleção de imagens para todas as páginas</t>
+  </si>
+  <si>
+    <t>LOGO: Elaboração do Logo</t>
+  </si>
+  <si>
+    <t>Próxima sprint</t>
+  </si>
+  <si>
+    <t>Separar HEAD, HEADER e FOOTER - e incluir nas páginas com php</t>
+  </si>
+  <si>
+    <t>PHP - tudo, nem sei por onde começar a listar isso.......</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +183,22 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -208,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -216,12 +280,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -233,6 +291,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,149 +580,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>43711</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>43725</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+        <v>43727</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="13"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
arquivos até a entrega da Sprint 2
</commit_message>
<xml_diff>
--- a/Projeto Integrador - Sprints.xlsx
+++ b/Projeto Integrador - Sprints.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Desktop\DIGITAL HOUSE\Curso Full Stack\Projeto-DH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE82EDF8-F040-466E-940B-5EC37428F6BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199FC2AE-0664-4CCA-BD6D-281BEA26974E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="kanban" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>SPRINT 1</t>
   </si>
@@ -136,13 +137,181 @@
   </si>
   <si>
     <t>PHP - tudo, nem sei por onde começar a listar isso.......</t>
+  </si>
+  <si>
+    <t>PROJETO INTEGRADOR - DIGITAL HOUSE</t>
+  </si>
+  <si>
+    <t>SolidarieVAGAS</t>
+  </si>
+  <si>
+    <t>PRONTO</t>
+  </si>
+  <si>
+    <t>FAZENDO</t>
+  </si>
+  <si>
+    <t>Legenda:</t>
+  </si>
+  <si>
+    <t>EM ANDAMENTO</t>
+  </si>
+  <si>
+    <t>NÃO INICIADO</t>
+  </si>
+  <si>
+    <t>AJUSTES FINAIS / TESTES</t>
+  </si>
+  <si>
+    <t>FINALIZADO</t>
+  </si>
+  <si>
+    <r>
+      <t>Atividade:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1) Logo e templates</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Responsável: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sabrine</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Data de entrega: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>25/09/2019</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Atividade:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2) Imagens e textos (para todas as páginas)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Responsável: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Stela</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Data de entrega: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>25/09/2019</t>
+    </r>
+  </si>
+  <si>
+    <t>ATIVIDADES</t>
+  </si>
+  <si>
+    <t>Início: 21/09/2019
+Prazo: 22/09/2019
+Entrega: 22/09/2019</t>
+  </si>
+  <si>
+    <t>OBS: Ajustes e aprovações de todos
+Início: 22/09/2019
+Prazo: 25/09/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prazo: 25/09/2019
+Entrega: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,8 +374,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +403,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -268,11 +482,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -291,15 +557,57 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,7 +890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -594,11 +902,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -630,11 +938,11 @@
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -702,7 +1010,7 @@
       <c r="C15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
@@ -716,7 +1024,7 @@
       <c r="B17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -724,7 +1032,7 @@
       <c r="B18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -732,16 +1040,16 @@
       <c r="B19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -845,4 +1153,189 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898C7F5C-0098-421B-A0C3-308A16D5091E}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="33.42578125" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="F1" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="F2" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="F3" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+    </row>
+    <row r="7" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+    </row>
+    <row r="9" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+    </row>
+    <row r="10" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+    </row>
+    <row r="11" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+    </row>
+    <row r="12" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+    </row>
+    <row r="17" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+    </row>
+    <row r="19" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+    </row>
+    <row r="21" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+    </row>
+    <row r="22" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+    </row>
+    <row r="23" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+    </row>
+    <row r="25" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+    </row>
+    <row r="26" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+    </row>
+    <row r="27" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+    </row>
+    <row r="28" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+    </row>
+    <row r="29" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+    </row>
+    <row r="30" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+    </row>
+    <row r="31" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>